<commit_message>
Delete Customer new commit
</commit_message>
<xml_diff>
--- a/FileInput/Customer Test Data.xlsx
+++ b/FileInput/Customer Test Data.xlsx
@@ -4,15 +4,21 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Admin Login" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Customer" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Add Customer" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Delete Customer" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="5j2hDwEi4MdOXS3QvqubOM8YHY43b9BsQXiLFidJZLU="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
   <si>
     <t>Username</t>
   </si>
@@ -74,7 +80,7 @@
     <t>4589657123</t>
   </si>
   <si>
-    <t>Seetha.Yadhu@gmail.com</t>
+    <t>Seetha.Raghu@gmail.com</t>
   </si>
   <si>
     <t>6987621476</t>
@@ -225,13 +231,25 @@
   </si>
   <si>
     <t>1 am a Carnatic Composer in Telugu!!</t>
+  </si>
+  <si>
+    <t>Customer No</t>
+  </si>
+  <si>
+    <t>Customer-00000011230</t>
+  </si>
+  <si>
+    <t>Customer-00000011231</t>
+  </si>
+  <si>
+    <t>Customer-00000011229</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -241,15 +259,24 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF747474"/>
+        <bgColor rgb="FF747474"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -258,14 +285,16 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -281,6 +310,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -486,9 +519,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,7 +532,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -520,245 +553,286 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="7" max="7" width="27.5"/>
     <col customWidth="1" min="9" max="9" width="31.88"/>
   </cols>
   <sheetData>
+    <row r="1" ht="15.75" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="18.88"/>
+  </cols>
+  <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>22</v>
+      <c r="A2" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>30</v>
+      <c r="A3" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>70</v>
+      <c r="A4" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in Apputil class to correct result excel file
</commit_message>
<xml_diff>
--- a/FileInput/Customer Test Data.xlsx
+++ b/FileInput/Customer Test Data.xlsx
@@ -236,20 +236,20 @@
     <t>Customer No</t>
   </si>
   <si>
-    <t>Customer-00000010026</t>
-  </si>
-  <si>
     <t>Customer-00000006849</t>
   </si>
   <si>
-    <t>Customer-00000010024</t>
+    <t>Customer-00000011271</t>
+  </si>
+  <si>
+    <t>Customer-00000011286</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -260,23 +260,13 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF747474"/>
-        <bgColor rgb="FF747474"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -285,15 +275,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -821,17 +808,17 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>